<commit_message>
Deploying to main from @ pedalboard/pedalboard-led-ring@e00b6006fbe5e0668d39e69566f899d81b2f64b9 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-led-ring-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-led-ring-bom.xlsx
@@ -440,7 +440,7 @@
     <t>Revision:</t>
   </si>
   <si>
-    <t>1.0.0</t>
+    <t>1.1.0-RC1</t>
   </si>
   <si>
     <t>Date:</t>
@@ -533,7 +533,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-10-17 15:15:15</t>
+    <t>2023-10-17 16:33:23</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-led-ring@60c8de256d417d4ea9619accf2f192840517f59a 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-led-ring-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-led-ring-bom.xlsx
@@ -264,7 +264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="98">
   <si>
     <t>Row</t>
   </si>
@@ -368,10 +368,10 @@
     <t>Conn_02x02_Odd_Even</t>
   </si>
   <si>
-    <t>J2</t>
-  </si>
-  <si>
-    <t>edge</t>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>middle</t>
   </si>
   <si>
     <t>PinSocket_2x02_P2.00mm_Vertical_SMD</t>
@@ -392,30 +392,15 @@
     <t>R</t>
   </si>
   <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>0</t>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>330</t>
   </si>
   <si>
     <t>R_0201_0603Metric_Pad0.64x0.40mm_HandSolder</t>
   </si>
   <si>
-    <t>https://industrial.panasonic.com/cdbs/www-data/pdf/RDA0000/AOA0000C301.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/en/products/detail/panasonic-electronic-components/ERJ-1GN0R00C/3982613</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>330</t>
-  </si>
-  <si>
     <t>https://api.pim.na.industrial.panasonic.com/file_stream/main/fileversion/1242</t>
   </si>
   <si>
@@ -461,13 +446,13 @@
     <t>Component Count:</t>
   </si>
   <si>
-    <t>29 (29 SMD/ 0 THT)</t>
+    <t>27 (27 SMD/ 0 THT)</t>
   </si>
   <si>
     <t>Fitted Components:</t>
   </si>
   <si>
-    <t>27 (27 SMD/ 0 THT)</t>
+    <t>26 (26 SMD/ 0 THT)</t>
   </si>
   <si>
     <t>Number of PCBs:</t>
@@ -500,12 +485,6 @@
     <t>1=K 2=A</t>
   </si>
   <si>
-    <t>J1</t>
-  </si>
-  <si>
-    <t>middle</t>
-  </si>
-  <si>
     <t>Global Part Info</t>
   </si>
   <si>
@@ -533,7 +512,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-10-17 16:33:23</t>
+    <t>2023-10-17 18:19:29</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>
@@ -1085,8 +1064,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>950034</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>168984</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>123779</xdr:rowOff>
     </xdr:to>
@@ -1412,7 +1391,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -1437,7 +1416,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1451,55 +1430,55 @@
     </row>
     <row r="2" spans="1:12">
       <c r="C2" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F2" s="3">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="C3" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="C4" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="C5" s="2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1507,16 +1486,16 @@
     </row>
     <row r="6" spans="1:12">
       <c r="C6" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="F6" s="3">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1706,44 +1685,6 @@
         <v>22</v>
       </c>
       <c r="L12" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="30" customHeight="1">
-      <c r="A13" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="K13" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="L13" s="8" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1759,7 +1700,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -1769,14 +1710,14 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="60.7109375" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="44.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
     <col min="4" max="4" width="25.7109375" customWidth="1"/>
     <col min="5" max="5" width="19.7109375" customWidth="1"/>
-    <col min="6" max="6" width="40.7109375" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1"/>
     <col min="7" max="7" width="26.7109375" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" customWidth="1"/>
-    <col min="9" max="9" width="44.7109375" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" customWidth="1"/>
     <col min="10" max="10" width="60.7109375" customWidth="1"/>
     <col min="11" max="11" width="20.7109375" customWidth="1"/>
     <col min="12" max="12" width="18.7109375" customWidth="1"/>
@@ -1784,7 +1725,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1798,55 +1739,55 @@
     </row>
     <row r="2" spans="1:12">
       <c r="C2" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F2" s="3">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="C3" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="C4" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="C5" s="2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1854,16 +1795,16 @@
     </row>
     <row r="6" spans="1:12">
       <c r="C6" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="F6" s="3">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1909,75 +1850,37 @@
         <v>12</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>12</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="I9" s="8" t="s">
         <v>22</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="45" customHeight="1">
-      <c r="A10" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="I10" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="J10" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="K10" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="L10" s="12" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1992,7 +1895,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="7" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
@@ -2014,7 +1917,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -2022,13 +1925,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -2036,13 +1939,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -2051,38 +1954,38 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G4" s="16">
-        <f>SUM(G10:G14)</f>
+        <f>SUM(G10:G13)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -2102,16 +2005,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1">
@@ -2202,39 +2105,17 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="30" customHeight="1">
-      <c r="A14" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="C14" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="E14" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
-      </c>
-      <c r="G14" s="20">
-        <f>IF(AND(ISNUMBER(E14),ISNUMBER(F14)),E14*F14,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="B17" s="22" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="23" t="s">
-        <v>90</v>
+    <row r="16" spans="1:7">
+      <c r="A16" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="23" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -2262,27 +2143,21 @@
       <formula>AND(ISBLANK(D13),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E14">
-    <cfRule type="expression" dxfId="0" priority="5">
-      <formula>AND(ISBLANK(D14),TRUE())</formula>
-    </cfRule>
-  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="D10" r:id="rId1"/>
     <hyperlink ref="D11" r:id="rId2"/>
     <hyperlink ref="D12" r:id="rId3"/>
     <hyperlink ref="D13" r:id="rId4"/>
-    <hyperlink ref="D14" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId6"/>
-  <legacyDrawing r:id="rId7"/>
+  <drawing r:id="rId5"/>
+  <legacyDrawing r:id="rId6"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="7" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
@@ -2295,8 +2170,8 @@
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" customWidth="1"/>
-    <col min="3" max="3" width="36.7109375" customWidth="1" outlineLevel="2"/>
-    <col min="4" max="4" width="40.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1" outlineLevel="2"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1" outlineLevel="1"/>
     <col min="5" max="5" width="26.7109375" customWidth="1" outlineLevel="1"/>
     <col min="6" max="6" width="15.7109375" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" customWidth="1"/>
@@ -2304,7 +2179,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -2312,13 +2187,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -2326,13 +2201,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -2341,38 +2216,38 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G4" s="16">
-        <f>SUM(G10:G11)</f>
+        <f>SUM(G10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -2392,27 +2267,27 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="19" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E10" s="19">
         <f>BoardQty*1</f>
@@ -2423,39 +2298,17 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
-      </c>
-      <c r="G11" s="20">
-        <f>IF(AND(ISNUMBER(E11),ISNUMBER(F11)),E11*F11,"")</f>
-        <v/>
+    <row r="13" spans="1:7">
+      <c r="A13" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="B14" s="22" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="23" t="s">
-        <v>90</v>
+      <c r="A14" s="23" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -2468,17 +2321,9 @@
       <formula>AND(ISBLANK(D10),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E11">
-    <cfRule type="expression" dxfId="0" priority="2">
-      <formula>AND(ISBLANK(D11),TRUE())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <hyperlinks>
-    <hyperlink ref="D11" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2495,72 +2340,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-led-ring@b5b77418c370e0f5f82283f9bb14bcc464b3174d 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-led-ring-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-led-ring-bom.xlsx
@@ -317,7 +317,7 @@
     <t>1uF</t>
   </si>
   <si>
-    <t>C_0201_0603Metric_Pad0.64x0.40mm_HandSolder</t>
+    <t>C_0402_1005Metric</t>
   </si>
   <si>
     <t>12</t>
@@ -371,7 +371,7 @@
     <t>J1</t>
   </si>
   <si>
-    <t>middle</t>
+    <t>02x02</t>
   </si>
   <si>
     <t>PinSocket_2x02_P2.00mm_Vertical_SMD</t>
@@ -398,7 +398,7 @@
     <t>330</t>
   </si>
   <si>
-    <t>R_0201_0603Metric_Pad0.64x0.40mm_HandSolder</t>
+    <t>R_0402_1005Metric</t>
   </si>
   <si>
     <t>https://api.pim.na.industrial.panasonic.com/file_stream/main/fileversion/1242</t>
@@ -512,7 +512,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-10-20 09:27:55</t>
+    <t>2023-10-21 09:13:57</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>
@@ -1405,7 +1405,7 @@
     <col min="3" max="3" width="24.7109375" customWidth="1"/>
     <col min="4" max="4" width="43.7109375" customWidth="1"/>
     <col min="5" max="5" width="19.7109375" customWidth="1"/>
-    <col min="6" max="6" width="48.7109375" customWidth="1"/>
+    <col min="6" max="6" width="40.7109375" customWidth="1"/>
     <col min="7" max="7" width="26.7109375" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" customWidth="1"/>
     <col min="9" max="9" width="60.7109375" customWidth="1"/>
@@ -1908,7 +1908,7 @@
   <cols>
     <col min="1" max="1" width="39.7109375" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="44.7109375" customWidth="1" outlineLevel="2"/>
+    <col min="3" max="3" width="36.7109375" customWidth="1" outlineLevel="2"/>
     <col min="4" max="4" width="61.7109375" customWidth="1" outlineLevel="1"/>
     <col min="5" max="5" width="26.7109375" customWidth="1" outlineLevel="1"/>
     <col min="6" max="6" width="15.7109375" customWidth="1"/>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-led-ring@3b04f1e66d0e252f5ea4c38dd57e18970d054831 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-led-ring-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-led-ring-bom.xlsx
@@ -264,7 +264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="99">
   <si>
     <t>Row</t>
   </si>
@@ -329,7 +329,7 @@
     <t>https://media.digikey.com/pdf/Data%20Sheets/Samsung%20PDFs/CL_Series_MLCC_ds.pdf</t>
   </si>
   <si>
-    <t>https://www.digikey.ch/en/products/detail/samsung-electro-mechanics/CL03A105MQ3CSNH/3894097</t>
+    <t>https://www.digikey.ch/de/products/detail/samsung-electro-mechanics/CL05A105KP5NNNC/3886734</t>
   </si>
   <si>
     <t/>
@@ -353,7 +353,7 @@
     <t>LED_SK6812_EC15_1.5x1.5mm</t>
   </si>
   <si>
-    <t>http://www.normandled.com/upload/202112/SK9810-EC15%20LED%20Datasheet.pdf</t>
+    <t>https://mm.digikey.com/Volume0/opasdata/d220001/medias/docus/2384/CL05A105KP5NNN_Specsheet%20(1).pdf</t>
   </si>
   <si>
     <t>https://www.digikey.ch/en/products/detail/adafruit-industries-llc/4492/11569136</t>
@@ -377,10 +377,10 @@
     <t>PinSocket_2x02_P2.00mm_Vertical_SMD</t>
   </si>
   <si>
-    <t>https://gct.co/files/drawings/bf100.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/en/products/detail/gct/BF100-04-A-D-1-0640-L-C/16396866</t>
+    <t>https://www.we-online.com/components/products/datasheet/621004242921.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/en/products/detail/w%C3%BCrth-elektronik/621004242921/15672146</t>
   </si>
   <si>
     <t>4</t>
@@ -401,10 +401,10 @@
     <t>R_0402_1005Metric</t>
   </si>
   <si>
-    <t>https://api.pim.na.industrial.panasonic.com/file_stream/main/fileversion/1242</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/en/products/detail/panasonic-electronic-components/ERJ-1GNJ331C/2035775</t>
+    <t>https://www.passivecomponent.com/wp-content/uploads/chipR/ASC_WR.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/en/products/detail/walsin-technology-corporation/WR04X3300FTL/13239224</t>
   </si>
   <si>
     <t>KiBot Bill of Materials</t>
@@ -476,6 +476,9 @@
     <t xml:space="preserve"> (DNF)</t>
   </si>
   <si>
+    <t>https://www.onsemi.com/pdf/datasheet/nsr05t40p2-d.pdf</t>
+  </si>
+  <si>
     <t>https://www.digikey.ch/de/products/detail/onsemi/NSR05T40P2T5G/5761753</t>
   </si>
   <si>
@@ -512,7 +515,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-10-21 15:35:09</t>
+    <t>2023-10-21 16:29:33</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>
@@ -1717,7 +1720,7 @@
     <col min="6" max="6" width="19.7109375" customWidth="1"/>
     <col min="7" max="7" width="26.7109375" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" customWidth="1"/>
-    <col min="9" max="9" width="19.7109375" customWidth="1"/>
+    <col min="9" max="9" width="58.7109375" customWidth="1"/>
     <col min="10" max="10" width="60.7109375" customWidth="1"/>
     <col min="11" max="11" width="20.7109375" customWidth="1"/>
     <col min="12" max="12" width="18.7109375" customWidth="1"/>
@@ -1870,17 +1873,17 @@
       <c r="H9" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="I9" s="8" t="s">
-        <v>22</v>
+      <c r="I9" s="7" t="s">
+        <v>70</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1931,7 +1934,7 @@
         <v>49</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -1945,7 +1948,7 @@
         <v>51</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -1960,7 +1963,7 @@
         <v>53</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G13)</f>
@@ -1985,7 +1988,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -2005,16 +2008,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1">
@@ -2061,7 +2064,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" ht="30" customHeight="1">
       <c r="A12" s="19" t="s">
         <v>34</v>
       </c>
@@ -2107,15 +2110,15 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="21" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="23" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -2171,7 +2174,7 @@
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" customWidth="1" outlineLevel="2"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="54.7109375" customWidth="1" outlineLevel="1"/>
     <col min="5" max="5" width="26.7109375" customWidth="1" outlineLevel="1"/>
     <col min="6" max="6" width="15.7109375" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" customWidth="1"/>
@@ -2193,7 +2196,7 @@
         <v>49</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -2207,7 +2210,7 @@
         <v>51</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -2222,7 +2225,7 @@
         <v>53</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10)</f>
@@ -2247,7 +2250,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -2267,16 +2270,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -2289,6 +2292,9 @@
       <c r="C10" s="19" t="s">
         <v>68</v>
       </c>
+      <c r="D10" s="19" t="s">
+        <v>70</v>
+      </c>
       <c r="E10" s="19">
         <f>BoardQty*1</f>
         <v>1</v>
@@ -2300,15 +2306,15 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="21" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="23" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -2321,9 +2327,12 @@
       <formula>AND(ISBLANK(D10),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="D10" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -2340,72 +2349,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-led-ring@ba03a3b744b5c1251bf5fb0e386ffec397c126ec 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-led-ring-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-led-ring-bom.xlsx
@@ -437,7 +437,7 @@
     <t>KiCad Version:</t>
   </si>
   <si>
-    <t>7.0.8-7.0.8~ubuntu23.04.1</t>
+    <t>7.0.9-7.0.9~ubuntu23.04.1</t>
   </si>
   <si>
     <t>Component Groups:</t>
@@ -515,7 +515,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-10-22 13:46:32</t>
+    <t>2024-01-08 21:15:21</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-led-ring@50576a36790cc6305b540b4fe3f144ed9e308a5f 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-led-ring-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-led-ring-bom.xlsx
@@ -515,10 +515,10 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2024-01-08 22:12:39</t>
-  </si>
-  <si>
-    <t>KiCost® v1.1.18 + KiBot v1.6.3</t>
+    <t>2024-01-10 19:27:33</t>
+  </si>
+  <si>
+    <t>KiCost® v1.1.18 + KiBot v1.6.4</t>
   </si>
   <si>
     <t>KiCad Fields (default)</t>

</xml_diff>